<commit_message>
Updated with new test countries and added requirements.txt folder
</commit_message>
<xml_diff>
--- a/Neural_Networks/Final Predictions/NNEU.xlsx
+++ b/Neural_Networks/Final Predictions/NNEU.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +441,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>country (nominal)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>population (discrete data)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>tests (discrete data)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Gini (discrete data)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>%urban pop. (continuous data)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Actual cases</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Pop*1.1</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Neural network Predictions EU</t>
         </is>
@@ -487,31 +497,37 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Albania</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>2875589</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>506676</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>0.637</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>61</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>117474</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>3163147.9</v>
       </c>
-      <c r="J2" t="n">
-        <v>256686.9996005073</v>
+      <c r="L2" t="n">
+        <v>251563.217744533</v>
       </c>
     </row>
     <row r="3">
@@ -521,31 +537,37 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Austria</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="F3" t="n">
         <v>9042407</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>6033827</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>0.739</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>59</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>495464</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>9946647.699999999</v>
       </c>
-      <c r="J3" t="n">
-        <v>522424.253499195</v>
+      <c r="L3" t="n">
+        <v>576226.2339787334</v>
       </c>
     </row>
     <row r="4">
@@ -555,31 +577,37 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Belgium</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="F4" t="n">
         <v>11624988</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>10110146</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>0.603</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>98</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>808283</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>12787486.8</v>
       </c>
-      <c r="J4" t="n">
-        <v>533300.3711652011</v>
+      <c r="L4" t="n">
+        <v>633231.994541347</v>
       </c>
     </row>
     <row r="5">
@@ -589,31 +617,37 @@
       <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>Bosnia and Herzegovina</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="F5" t="n">
         <v>3266449</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>702920</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>0.642</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>49</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>142160</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>3593093.9</v>
       </c>
-      <c r="J5" t="n">
-        <v>266252.9985946082</v>
+      <c r="L5" t="n">
+        <v>278434.3786247783</v>
       </c>
     </row>
     <row r="6">
@@ -623,31 +657,37 @@
       <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Croatia</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="F6" t="n">
         <v>4087440</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
         <v>1431342</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
         <v>0.645</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>57</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>251174</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>4496184</v>
       </c>
-      <c r="J6" t="n">
-        <v>333051.1029542015</v>
+      <c r="L6" t="n">
+        <v>333944.0034979284</v>
       </c>
     </row>
     <row r="7">
@@ -657,31 +697,37 @@
       <c r="B7" t="n">
         <v>5</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Cyprus</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="F7" t="n">
         <v>1213513</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
         <v>2563270</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>0.801</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>67</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>39651</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>1334864.3</v>
       </c>
-      <c r="J7" t="n">
-        <v>176089.5003415607</v>
+      <c r="L7" t="n">
+        <v>176817.9465027489</v>
       </c>
     </row>
     <row r="8">
@@ -691,31 +737,37 @@
       <c r="B8" t="n">
         <v>6</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>Czechia</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="F8" t="n">
         <v>10722926</v>
       </c>
-      <c r="E8" t="n">
+      <c r="G8" t="n">
         <v>9665502</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>0.725</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>74</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>1402420</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>11795218.6</v>
       </c>
-      <c r="J8" t="n">
-        <v>615542.3985333294</v>
+      <c r="L8" t="n">
+        <v>655508.4596501142</v>
       </c>
     </row>
     <row r="9">
@@ -725,31 +777,37 @@
       <c r="B9" t="n">
         <v>7</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Denmark</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="F9" t="n">
         <v>5806809</v>
       </c>
-      <c r="E9" t="n">
+      <c r="G9" t="n">
         <v>20418687</v>
       </c>
-      <c r="F9" t="n">
+      <c r="H9" t="n">
         <v>0.838</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>88</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>220459</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>6387489.9</v>
       </c>
-      <c r="J9" t="n">
-        <v>304328.9815952555</v>
+      <c r="L9" t="n">
+        <v>296740.7571483479</v>
       </c>
     </row>
     <row r="10">
@@ -759,31 +817,37 @@
       <c r="B10" t="n">
         <v>8</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>Estonia</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="F10" t="n">
         <v>1327161</v>
       </c>
-      <c r="E10" t="n">
+      <c r="G10" t="n">
         <v>1038888</v>
       </c>
-      <c r="F10" t="n">
+      <c r="H10" t="n">
         <v>0.716</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>69</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>86086</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>1459877.1</v>
       </c>
-      <c r="J10" t="n">
-        <v>151975.1742120292</v>
+      <c r="L10" t="n">
+        <v>138919.7688018773</v>
       </c>
     </row>
     <row r="11">
@@ -793,31 +857,37 @@
       <c r="B11" t="n">
         <v>9</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Finland</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="F11" t="n">
         <v>5546762</v>
       </c>
-      <c r="E11" t="n">
+      <c r="G11" t="n">
         <v>3596402</v>
       </c>
-      <c r="F11" t="n">
+      <c r="H11" t="n">
         <v>0.742</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>85</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>67334</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>6101438.2</v>
       </c>
-      <c r="J11" t="n">
-        <v>296982.1423606389</v>
+      <c r="L11" t="n">
+        <v>319701.7887703628</v>
       </c>
     </row>
     <row r="12">
@@ -827,31 +897,37 @@
       <c r="B12" t="n">
         <v>10</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>France</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="F12" t="n">
         <v>65374874</v>
       </c>
-      <c r="E12" t="n">
+      <c r="G12" t="n">
         <v>57231533</v>
       </c>
-      <c r="F12" t="n">
+      <c r="H12" t="n">
         <v>0.696</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>81</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>4071662</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>71912361.40000001</v>
       </c>
-      <c r="J12" t="n">
-        <v>2972790.215654314</v>
+      <c r="L12" t="n">
+        <v>3497310.176442087</v>
       </c>
     </row>
     <row r="13">
@@ -861,31 +937,37 @@
       <c r="B13" t="n">
         <v>11</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Germany</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="F13" t="n">
         <v>83971874</v>
       </c>
-      <c r="E13" t="n">
+      <c r="G13" t="n">
         <v>46319641</v>
       </c>
-      <c r="F13" t="n">
+      <c r="H13" t="n">
         <v>0.8159999999999999</v>
       </c>
-      <c r="G13" t="n">
+      <c r="I13" t="n">
         <v>77</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>2578835</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="n">
         <v>92369061.40000001</v>
       </c>
-      <c r="J13" t="n">
-        <v>3656004.883702517</v>
+      <c r="L13" t="n">
+        <v>4327824.673547745</v>
       </c>
     </row>
     <row r="14">
@@ -895,31 +977,37 @@
       <c r="B14" t="n">
         <v>12</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>Greece</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="F14" t="n">
         <v>10387221</v>
       </c>
-      <c r="E14" t="n">
+      <c r="G14" t="n">
         <v>5856618</v>
       </c>
-      <c r="F14" t="n">
+      <c r="H14" t="n">
         <v>0.654</v>
       </c>
-      <c r="G14" t="n">
+      <c r="I14" t="n">
         <v>79</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>221147</v>
       </c>
-      <c r="I14" t="n">
+      <c r="K14" t="n">
         <v>11425943.1</v>
       </c>
-      <c r="J14" t="n">
-        <v>589824.0842487216</v>
+      <c r="L14" t="n">
+        <v>650919.0130915344</v>
       </c>
     </row>
     <row r="15">
@@ -929,31 +1017,37 @@
       <c r="B15" t="n">
         <v>13</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>Hungary</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="F15" t="n">
         <v>9643103</v>
       </c>
-      <c r="E15" t="n">
+      <c r="G15" t="n">
         <v>4104415</v>
       </c>
-      <c r="F15" t="n">
+      <c r="H15" t="n">
         <v>0.663</v>
       </c>
-      <c r="G15" t="n">
+      <c r="I15" t="n">
         <v>72</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>524196</v>
       </c>
-      <c r="I15" t="n">
+      <c r="K15" t="n">
         <v>10607413.3</v>
       </c>
-      <c r="J15" t="n">
-        <v>588992.2568826079</v>
+      <c r="L15" t="n">
+        <v>634743.8935857117</v>
       </c>
     </row>
     <row r="16">
@@ -963,31 +1057,37 @@
       <c r="B16" t="n">
         <v>14</v>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Ireland</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="F16" t="n">
         <v>4976339</v>
       </c>
-      <c r="E16" t="n">
+      <c r="G16" t="n">
         <v>3720861</v>
       </c>
-      <c r="F16" t="n">
+      <c r="H16" t="n">
         <v>0.796</v>
       </c>
-      <c r="G16" t="n">
+      <c r="I16" t="n">
         <v>63</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>225741</v>
       </c>
-      <c r="I16" t="n">
+      <c r="K16" t="n">
         <v>5473972.9</v>
       </c>
-      <c r="J16" t="n">
-        <v>344260.9385444075</v>
+      <c r="L16" t="n">
+        <v>377138.9906278402</v>
       </c>
     </row>
     <row r="17">
@@ -997,31 +1097,37 @@
       <c r="B17" t="n">
         <v>15</v>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="F17" t="n">
         <v>60399338</v>
       </c>
-      <c r="E17" t="n">
+      <c r="G17" t="n">
         <v>44623304</v>
       </c>
-      <c r="F17" t="n">
+      <c r="H17" t="n">
         <v>0.669</v>
       </c>
-      <c r="G17" t="n">
+      <c r="I17" t="n">
         <v>71</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>3223142</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="n">
         <v>66439271.8</v>
       </c>
-      <c r="J17" t="n">
-        <v>2670484.587275029</v>
+      <c r="L17" t="n">
+        <v>3198625.813449562</v>
       </c>
     </row>
     <row r="18">
@@ -1031,31 +1137,37 @@
       <c r="B18" t="n">
         <v>16</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>Latvia</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="F18" t="n">
         <v>1871486</v>
       </c>
-      <c r="E18" t="n">
+      <c r="G18" t="n">
         <v>1670193</v>
       </c>
-      <c r="F18" t="n">
+      <c r="H18" t="n">
         <v>0.789</v>
       </c>
-      <c r="G18" t="n">
+      <c r="I18" t="n">
         <v>68</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>93959</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
         <v>2058634.6</v>
       </c>
-      <c r="J18" t="n">
-        <v>196933.7475718148</v>
+      <c r="L18" t="n">
+        <v>192016.3980853595</v>
       </c>
     </row>
     <row r="19">
@@ -1065,31 +1177,37 @@
       <c r="B19" t="n">
         <v>17</v>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Lithuania</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="F19" t="n">
         <v>2695463</v>
       </c>
-      <c r="E19" t="n">
+      <c r="G19" t="n">
         <v>2218746</v>
       </c>
-      <c r="F19" t="n">
+      <c r="H19" t="n">
         <v>0.663</v>
       </c>
-      <c r="G19" t="n">
+      <c r="I19" t="n">
         <v>68</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>205644</v>
       </c>
-      <c r="I19" t="n">
+      <c r="K19" t="n">
         <v>2965009.3</v>
       </c>
-      <c r="J19" t="n">
-        <v>211030.5088102371</v>
+      <c r="L19" t="n">
+        <v>215133.8216760904</v>
       </c>
     </row>
     <row r="20">
@@ -1099,31 +1217,37 @@
       <c r="B20" t="n">
         <v>18</v>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" t="n">
+        <v>18</v>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>Luxembourg</t>
         </is>
       </c>
-      <c r="D20" t="n">
+      <c r="F20" t="n">
         <v>633079</v>
       </c>
-      <c r="E20" t="n">
+      <c r="G20" t="n">
         <v>2248588</v>
       </c>
-      <c r="F20" t="n">
+      <c r="H20" t="n">
         <v>0.67</v>
       </c>
-      <c r="G20" t="n">
+      <c r="I20" t="n">
         <v>91</v>
       </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
         <v>57877</v>
       </c>
-      <c r="I20" t="n">
+      <c r="K20" t="n">
         <v>696386.9</v>
       </c>
-      <c r="J20" t="n">
-        <v>20491.86208807444</v>
+      <c r="L20" t="n">
+        <v>119055.686350733</v>
       </c>
     </row>
     <row r="21">
@@ -1133,31 +1257,37 @@
       <c r="B21" t="n">
         <v>19</v>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" t="n">
+        <v>19</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Moldova</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="F21" t="n">
         <v>4027371</v>
       </c>
-      <c r="E21" t="n">
+      <c r="G21" t="n">
         <v>771763</v>
       </c>
-      <c r="F21" t="n">
+      <c r="H21" t="n">
         <v>0.645</v>
       </c>
-      <c r="G21" t="n">
+      <c r="I21" t="n">
         <v>43</v>
       </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
         <v>204463</v>
       </c>
-      <c r="I21" t="n">
+      <c r="K21" t="n">
         <v>4430108.100000001</v>
       </c>
-      <c r="J21" t="n">
-        <v>251331.6237287559</v>
+      <c r="L21" t="n">
+        <v>207012.0477421023</v>
       </c>
     </row>
     <row r="22">
@@ -1167,31 +1297,37 @@
       <c r="B22" t="n">
         <v>20</v>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>Netherlands</t>
         </is>
       </c>
-      <c r="D22" t="n">
+      <c r="F22" t="n">
         <v>17161479</v>
       </c>
-      <c r="E22" t="n">
+      <c r="G22" t="n">
         <v>6970400</v>
       </c>
-      <c r="F22" t="n">
+      <c r="H22" t="n">
         <v>0.902</v>
       </c>
-      <c r="G22" t="n">
+      <c r="I22" t="n">
         <v>92</v>
       </c>
-      <c r="H22" t="n">
+      <c r="J22" t="n">
         <v>1157192</v>
       </c>
-      <c r="I22" t="n">
+      <c r="K22" t="n">
         <v>18877626.9</v>
       </c>
-      <c r="J22" t="n">
-        <v>845405.745674625</v>
+      <c r="L22" t="n">
+        <v>916409.9940377772</v>
       </c>
     </row>
     <row r="23">
@@ -1201,31 +1337,37 @@
       <c r="B23" t="n">
         <v>21</v>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>Norway</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="F23" t="n">
         <v>5450917</v>
       </c>
-      <c r="E23" t="n">
+      <c r="G23" t="n">
         <v>4115415</v>
       </c>
-      <c r="F23" t="n">
+      <c r="H23" t="n">
         <v>0.798</v>
       </c>
-      <c r="G23" t="n">
+      <c r="I23" t="n">
         <v>83</v>
       </c>
-      <c r="H23" t="n">
+      <c r="J23" t="n">
         <v>80440</v>
       </c>
-      <c r="I23" t="n">
+      <c r="K23" t="n">
         <v>5996008.7</v>
       </c>
-      <c r="J23" t="n">
-        <v>300359.570806928</v>
+      <c r="L23" t="n">
+        <v>296354.6099599898</v>
       </c>
     </row>
     <row r="24">
@@ -1235,31 +1377,37 @@
       <c r="B24" t="n">
         <v>22</v>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="C24" t="n">
+        <v>22</v>
+      </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>Poland</t>
         </is>
       </c>
-      <c r="D24" t="n">
+      <c r="F24" t="n">
         <v>37817481</v>
       </c>
-      <c r="E24" t="n">
+      <c r="G24" t="n">
         <v>10668987</v>
       </c>
-      <c r="F24" t="n">
+      <c r="H24" t="n">
         <v>0.677</v>
       </c>
-      <c r="G24" t="n">
+      <c r="I24" t="n">
         <v>60</v>
       </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
         <v>1917527</v>
       </c>
-      <c r="I24" t="n">
+      <c r="K24" t="n">
         <v>41599229.1</v>
       </c>
-      <c r="J24" t="n">
-        <v>1781236.992806673</v>
+      <c r="L24" t="n">
+        <v>2041676.78505376</v>
       </c>
     </row>
     <row r="25">
@@ -1269,31 +1417,37 @@
       <c r="B25" t="n">
         <v>23</v>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C25" t="n">
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>Portugal</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="F25" t="n">
         <v>10175800</v>
       </c>
-      <c r="E25" t="n">
+      <c r="G25" t="n">
         <v>8480932</v>
       </c>
-      <c r="F25" t="n">
+      <c r="H25" t="n">
         <v>0.6919999999999999</v>
       </c>
-      <c r="G25" t="n">
+      <c r="I25" t="n">
         <v>66</v>
       </c>
-      <c r="H25" t="n">
+      <c r="J25" t="n">
         <v>814257</v>
       </c>
-      <c r="I25" t="n">
+      <c r="K25" t="n">
         <v>11193380</v>
       </c>
-      <c r="J25" t="n">
-        <v>613184.5275371969</v>
+      <c r="L25" t="n">
+        <v>650124.9046204984</v>
       </c>
     </row>
     <row r="26">
@@ -1303,31 +1457,37 @@
       <c r="B26" t="n">
         <v>24</v>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="C26" t="n">
+        <v>24</v>
+      </c>
+      <c r="D26" t="n">
+        <v>24</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>Romania</t>
         </is>
       </c>
-      <c r="D26" t="n">
+      <c r="F26" t="n">
         <v>19147305</v>
       </c>
-      <c r="E26" t="n">
+      <c r="G26" t="n">
         <v>6774562</v>
       </c>
-      <c r="F26" t="n">
+      <c r="H26" t="n">
         <v>0.647</v>
       </c>
-      <c r="G26" t="n">
+      <c r="I26" t="n">
         <v>54</v>
       </c>
-      <c r="H26" t="n">
+      <c r="J26" t="n">
         <v>862681</v>
       </c>
-      <c r="I26" t="n">
+      <c r="K26" t="n">
         <v>21062035.5</v>
       </c>
-      <c r="J26" t="n">
-        <v>997680.6969928294</v>
+      <c r="L26" t="n">
+        <v>1107718.343927145</v>
       </c>
     </row>
     <row r="27">
@@ -1337,31 +1497,37 @@
       <c r="B27" t="n">
         <v>25</v>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="C27" t="n">
+        <v>25</v>
+      </c>
+      <c r="D27" t="n">
+        <v>25</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>Serbia</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="F27" t="n">
         <v>8712609</v>
       </c>
-      <c r="E27" t="n">
+      <c r="G27" t="n">
         <v>3149048</v>
       </c>
-      <c r="F27" t="n">
+      <c r="H27" t="n">
         <v>0.676</v>
       </c>
-      <c r="G27" t="n">
+      <c r="I27" t="n">
         <v>56</v>
       </c>
-      <c r="H27" t="n">
+      <c r="J27" t="n">
         <v>516277</v>
       </c>
-      <c r="I27" t="n">
+      <c r="K27" t="n">
         <v>9583869.9</v>
       </c>
-      <c r="J27" t="n">
-        <v>539408.8833582103</v>
+      <c r="L27" t="n">
+        <v>571739.0056258142</v>
       </c>
     </row>
     <row r="28">
@@ -1371,31 +1537,37 @@
       <c r="B28" t="n">
         <v>26</v>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C28" t="n">
+        <v>26</v>
+      </c>
+      <c r="D28" t="n">
+        <v>26</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>Slovak Republic</t>
         </is>
       </c>
-      <c r="D28" t="n">
+      <c r="F28" t="n">
         <v>5461499</v>
       </c>
-      <c r="E28" t="n">
+      <c r="G28" t="n">
         <v>2200380</v>
       </c>
-      <c r="F28" t="n">
+      <c r="H28" t="n">
         <v>0.498</v>
       </c>
-      <c r="G28" t="n">
+      <c r="I28" t="n">
         <v>54</v>
       </c>
-      <c r="H28" t="n">
+      <c r="J28" t="n">
         <v>337960</v>
       </c>
-      <c r="I28" t="n">
+      <c r="K28" t="n">
         <v>6007648.9</v>
       </c>
-      <c r="J28" t="n">
-        <v>398343.3275764362</v>
+      <c r="L28" t="n">
+        <v>399140.7993156165</v>
       </c>
     </row>
     <row r="29">
@@ -1405,31 +1577,37 @@
       <c r="B29" t="n">
         <v>27</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>Slovenia</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="F29" t="n">
         <v>2079139</v>
       </c>
-      <c r="E29" t="n">
+      <c r="G29" t="n">
         <v>976907</v>
       </c>
-      <c r="F29" t="n">
+      <c r="H29" t="n">
         <v>0.662</v>
       </c>
-      <c r="G29" t="n">
+      <c r="I29" t="n">
         <v>55</v>
       </c>
-      <c r="H29" t="n">
+      <c r="J29" t="n">
         <v>200579</v>
       </c>
-      <c r="I29" t="n">
+      <c r="K29" t="n">
         <v>2287052.9</v>
       </c>
-      <c r="J29" t="n">
-        <v>228463.0191158876</v>
+      <c r="L29" t="n">
+        <v>244961.4995659702</v>
       </c>
     </row>
     <row r="30">
@@ -1439,31 +1617,37 @@
       <c r="B30" t="n">
         <v>28</v>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="C30" t="n">
+        <v>28</v>
+      </c>
+      <c r="D30" t="n">
+        <v>28</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>Spain</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="F30" t="n">
         <v>46767497</v>
       </c>
-      <c r="E30" t="n">
+      <c r="G30" t="n">
         <v>40292390</v>
       </c>
-      <c r="F30" t="n">
+      <c r="H30" t="n">
         <v>0.694</v>
       </c>
-      <c r="G30" t="n">
+      <c r="I30" t="n">
         <v>81</v>
       </c>
-      <c r="H30" t="n">
+      <c r="J30" t="n">
         <v>3183704</v>
       </c>
-      <c r="I30" t="n">
+      <c r="K30" t="n">
         <v>51444246.7</v>
       </c>
-      <c r="J30" t="n">
-        <v>2233360.0607602</v>
+      <c r="L30" t="n">
+        <v>2585950.759841979</v>
       </c>
     </row>
     <row r="31">
@@ -1473,31 +1657,37 @@
       <c r="B31" t="n">
         <v>29</v>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="C31" t="n">
+        <v>29</v>
+      </c>
+      <c r="D31" t="n">
+        <v>29</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>Sweden</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="F31" t="n">
         <v>10143382</v>
       </c>
-      <c r="E31" t="n">
+      <c r="G31" t="n">
         <v>6627544</v>
       </c>
-      <c r="F31" t="n">
+      <c r="H31" t="n">
         <v>0.867</v>
       </c>
-      <c r="G31" t="n">
+      <c r="I31" t="n">
         <v>88</v>
       </c>
-      <c r="H31" t="n">
+      <c r="J31" t="n">
         <v>712527</v>
       </c>
-      <c r="I31" t="n">
+      <c r="K31" t="n">
         <v>11157720.2</v>
       </c>
-      <c r="J31" t="n">
-        <v>506398.940871656</v>
+      <c r="L31" t="n">
+        <v>526947.4405320883</v>
       </c>
     </row>
     <row r="32">
@@ -1507,31 +1697,37 @@
       <c r="B32" t="n">
         <v>30</v>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="C32" t="n">
+        <v>30</v>
+      </c>
+      <c r="D32" t="n">
+        <v>30</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>Switzerland</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="F32" t="n">
         <v>8698941</v>
       </c>
-      <c r="E32" t="n">
+      <c r="G32" t="n">
         <v>5387481</v>
       </c>
-      <c r="F32" t="n">
+      <c r="H32" t="n">
         <v>0.705</v>
       </c>
-      <c r="G32" t="n">
+      <c r="I32" t="n">
         <v>74</v>
       </c>
-      <c r="H32" t="n">
+      <c r="J32" t="n">
         <v>570645</v>
       </c>
-      <c r="I32" t="n">
+      <c r="K32" t="n">
         <v>9568835.1</v>
       </c>
-      <c r="J32" t="n">
-        <v>512362.2038862035</v>
+      <c r="L32" t="n">
+        <v>540337.8997439742</v>
       </c>
     </row>
     <row r="33">
@@ -1541,31 +1737,37 @@
       <c r="B33" t="n">
         <v>31</v>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="C33" t="n">
+        <v>31</v>
+      </c>
+      <c r="D33" t="n">
+        <v>31</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="D33" t="n">
+      <c r="F33" t="n">
         <v>68135945</v>
       </c>
-      <c r="E33" t="n">
+      <c r="G33" t="n">
         <v>103053938</v>
       </c>
-      <c r="F33" t="n">
+      <c r="H33" t="n">
         <v>0.746</v>
       </c>
-      <c r="G33" t="n">
+      <c r="I33" t="n">
         <v>84</v>
       </c>
-      <c r="H33" t="n">
+      <c r="J33" t="n">
         <v>4258438</v>
       </c>
-      <c r="I33" t="n">
+      <c r="K33" t="n">
         <v>74949539.5</v>
       </c>
-      <c r="J33" t="n">
-        <v>3111147.649066747</v>
+      <c r="L33" t="n">
+        <v>3659250.217435003</v>
       </c>
     </row>
     <row r="34">
@@ -1575,31 +1777,37 @@
       <c r="B34" t="n">
         <v>32</v>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C34" t="n">
+        <v>32</v>
+      </c>
+      <c r="D34" t="n">
+        <v>32</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>Ukraine</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="F34" t="n">
         <v>43548757</v>
       </c>
-      <c r="E34" t="n">
+      <c r="G34" t="n">
         <v>7328468</v>
       </c>
-      <c r="F34" t="n">
+      <c r="H34" t="n">
         <v>0.847</v>
       </c>
-      <c r="G34" t="n">
+      <c r="I34" t="n">
         <v>69</v>
       </c>
-      <c r="H34" t="n">
+      <c r="J34" t="n">
         <v>1467548</v>
       </c>
-      <c r="I34" t="n">
+      <c r="K34" t="n">
         <v>47903632.7</v>
       </c>
-      <c r="J34" t="n">
-        <v>2050481.255272448</v>
+      <c r="L34" t="n">
+        <v>2315501.504408122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>